<commit_message>
🚨 HOTFIX URGENTE: Eliminar error pre-cache + productos.json siempre fresh
❌ ERRORES ARREGLADOS:
- Eliminado precacheProductImages() que causaba error en consola F12
- productos.json ahora NUNCA se cachea - siempre fresh del servidor
- Service Worker v1.2.7 con cache busting forzado

✅ FUNCIONALIDAD RESTAURADA:
- Sin errores en consola
- Cambios en productos.json se ven inmediatamente
- Edición de cantidades en carrito mantiene funcionando
- Todo como estaba antes + mejora de cantidades

🔧 Solo se mantiene la edición de cantidades que funciona perfecto
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\mare-catalog-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84819A30-9BEB-453F-8963-57F88F6B4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608E9F14-917D-4B78-A6D8-F8E3AB139397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6337" uniqueCount="1955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6328" uniqueCount="1954">
   <si>
     <t>Código</t>
   </si>
@@ -5749,9 +5749,6 @@
   </si>
   <si>
     <t>Z Enchapado</t>
-  </si>
-  <si>
-    <t>BAG0172</t>
   </si>
   <si>
     <t>BAG1417</t>
@@ -6266,11 +6263,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM990"/>
+  <dimension ref="A1:BM989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A620" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A637" sqref="A637:XFD637"/>
+      <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A327" sqref="A327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8804,7 +8801,7 @@
     </row>
     <row r="43" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>332</v>
@@ -9573,7 +9570,7 @@
     </row>
     <row r="57" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>396</v>
@@ -9735,7 +9732,7 @@
         <v>485</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>1868</v>
@@ -9785,7 +9782,7 @@
         <v>492</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>1868</v>
@@ -9894,7 +9891,7 @@
     </row>
     <row r="63" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>507</v>
@@ -10115,7 +10112,7 @@
     </row>
     <row r="67" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>544</v>
@@ -10625,7 +10622,7 @@
     </row>
     <row r="78" spans="1:61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>607</v>
@@ -11434,7 +11431,7 @@
     </row>
     <row r="101" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>663</v>
@@ -14410,7 +14407,7 @@
         <v>1049</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>830</v>
@@ -20871,10 +20868,10 @@
         <v>1506</v>
       </c>
       <c r="B325" s="5" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C325" s="5" t="s">
         <v>1943</v>
-      </c>
-      <c r="C325" s="5" t="s">
-        <v>1944</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>1903</v>
@@ -20915,10 +20912,10 @@
         <v>1507</v>
       </c>
       <c r="B326" s="5" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C326" s="5" t="s">
         <v>1943</v>
-      </c>
-      <c r="C326" s="5" t="s">
-        <v>1944</v>
       </c>
       <c r="D326" s="2" t="s">
         <v>1903</v>
@@ -20948,10 +20945,10 @@
         <v>1508</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>1903</v>
@@ -29058,7 +29055,7 @@
     </row>
     <row r="548" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A548" s="15" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B548" s="5" t="s">
         <v>1832</v>
@@ -32608,7 +32605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="673" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A673">
         <v>14394</v>
       </c>
@@ -32635,7 +32632,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="674" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A674">
         <v>14395</v>
       </c>
@@ -32662,7 +32659,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="675" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>14396</v>
       </c>
@@ -32689,7 +32686,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="676" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A676">
         <v>73383</v>
       </c>
@@ -32716,7 +32713,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="677" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A677">
         <v>85713</v>
       </c>
@@ -32743,7 +32740,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="678" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A678">
         <v>14484</v>
       </c>
@@ -32770,7 +32767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="679" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A679">
         <v>77723</v>
       </c>
@@ -32797,7 +32794,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="680" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A680">
         <v>13594</v>
       </c>
@@ -32824,7 +32821,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="681" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A681">
         <v>14444</v>
       </c>
@@ -32851,7 +32848,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="682" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
         <v>1885</v>
       </c>
@@ -32878,7 +32875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="683" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>1887</v>
       </c>
@@ -32905,7 +32902,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="684" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A684">
         <v>252408</v>
       </c>
@@ -32932,7 +32929,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="685" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A685">
         <v>252407</v>
       </c>
@@ -32959,7 +32956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="686" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A686">
         <v>252406</v>
       </c>
@@ -32986,7 +32983,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="687" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A687">
         <v>252409</v>
       </c>
@@ -33013,7 +33010,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="688" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
         <v>1905</v>
       </c>
@@ -33035,34 +33032,10 @@
       <c r="H688">
         <v>2</v>
       </c>
-      <c r="I688">
-        <v>3</v>
-      </c>
-      <c r="J688">
-        <v>4</v>
-      </c>
-      <c r="K688">
-        <v>5</v>
-      </c>
-      <c r="L688">
-        <v>6</v>
-      </c>
-      <c r="M688">
-        <v>7</v>
-      </c>
-      <c r="S688" t="s">
-        <v>68</v>
-      </c>
       <c r="T688" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="U688" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK688" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN688" t="s">
+      <c r="AI688" t="s">
         <v>68</v>
       </c>
     </row>
@@ -33079,8 +33052,11 @@
       <c r="D689" s="5" t="s">
         <v>1867</v>
       </c>
+      <c r="E689" s="5" t="s">
+        <v>1907</v>
+      </c>
       <c r="F689" s="10">
-        <v>390</v>
+        <v>590</v>
       </c>
       <c r="G689" s="10">
         <v>1</v>
@@ -33088,31 +33064,43 @@
       <c r="H689">
         <v>2</v>
       </c>
+      <c r="I689">
+        <v>3</v>
+      </c>
+      <c r="J689">
+        <v>4</v>
+      </c>
+      <c r="S689" t="s">
+        <v>68</v>
+      </c>
       <c r="T689" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="AI689" t="s">
+      <c r="AH689" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT689" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="690" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="B690" s="5" t="s">
-        <v>331</v>
+        <v>1909</v>
       </c>
       <c r="C690" s="5" t="s">
-        <v>331</v>
+        <v>1909</v>
       </c>
       <c r="D690" s="5" t="s">
         <v>1867</v>
       </c>
       <c r="E690" s="5" t="s">
-        <v>1908</v>
+        <v>1910</v>
       </c>
       <c r="F690" s="10">
-        <v>590</v>
+        <v>120</v>
       </c>
       <c r="G690" s="10">
         <v>1</v>
@@ -33123,8 +33111,8 @@
       <c r="I690">
         <v>3</v>
       </c>
-      <c r="J690">
-        <v>4</v>
+      <c r="Q690">
+        <v>1</v>
       </c>
       <c r="S690" t="s">
         <v>68</v>
@@ -33132,31 +33120,25 @@
       <c r="T690" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="AH690" t="s">
-        <v>68</v>
-      </c>
-      <c r="AT690" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="691" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>1909</v>
+        <v>1911</v>
       </c>
       <c r="B691" s="5" t="s">
-        <v>1910</v>
+        <v>535</v>
       </c>
       <c r="C691" s="5" t="s">
-        <v>1910</v>
+        <v>537</v>
       </c>
       <c r="D691" s="5" t="s">
-        <v>1867</v>
+        <v>108</v>
       </c>
       <c r="E691" s="5" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="F691" s="10">
-        <v>120</v>
+        <v>395</v>
       </c>
       <c r="G691" s="10">
         <v>1</v>
@@ -33176,25 +33158,34 @@
       <c r="T691" s="5" t="s">
         <v>1888</v>
       </c>
+      <c r="U691" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE691" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW691" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="692" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="B692" s="5" t="s">
-        <v>535</v>
+        <v>331</v>
       </c>
       <c r="C692" s="5" t="s">
-        <v>537</v>
+        <v>331</v>
       </c>
       <c r="D692" s="5" t="s">
-        <v>108</v>
+        <v>1867</v>
       </c>
       <c r="E692" s="5" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="F692" s="10">
-        <v>395</v>
+        <v>490</v>
       </c>
       <c r="G692" s="10">
         <v>1</v>
@@ -33205,6 +33196,12 @@
       <c r="I692">
         <v>3</v>
       </c>
+      <c r="J692">
+        <v>4</v>
+      </c>
+      <c r="K692">
+        <v>5</v>
+      </c>
       <c r="Q692">
         <v>1</v>
       </c>
@@ -33214,7 +33211,10 @@
       <c r="T692" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="U692" t="s">
+      <c r="V692" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC692" t="s">
         <v>68</v>
       </c>
       <c r="AE692" t="s">
@@ -33226,7 +33226,7 @@
     </row>
     <row r="693" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
       <c r="B693" s="5" t="s">
         <v>331</v>
@@ -33238,7 +33238,7 @@
         <v>1867</v>
       </c>
       <c r="E693" s="5" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="F693" s="10">
         <v>490</v>
@@ -33255,9 +33255,6 @@
       <c r="J693">
         <v>4</v>
       </c>
-      <c r="K693">
-        <v>5</v>
-      </c>
       <c r="Q693">
         <v>1</v>
       </c>
@@ -33267,13 +33264,10 @@
       <c r="T693" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="V693" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC693" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE693" t="s">
+      <c r="U693" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD693" t="s">
         <v>68</v>
       </c>
       <c r="AW693" t="s">
@@ -33282,7 +33276,7 @@
     </row>
     <row r="694" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="B694" s="5" t="s">
         <v>331</v>
@@ -33294,10 +33288,10 @@
         <v>1867</v>
       </c>
       <c r="E694" s="5" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="F694" s="10">
-        <v>490</v>
+        <v>285</v>
       </c>
       <c r="G694" s="10">
         <v>1</v>
@@ -33308,9 +33302,6 @@
       <c r="I694">
         <v>3</v>
       </c>
-      <c r="J694">
-        <v>4</v>
-      </c>
       <c r="Q694">
         <v>1</v>
       </c>
@@ -33318,21 +33309,12 @@
         <v>68</v>
       </c>
       <c r="T694" s="5" t="s">
-        <v>1888</v>
-      </c>
-      <c r="U694" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD694" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW694" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="695" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="B695" s="5" t="s">
         <v>331</v>
@@ -33344,10 +33326,10 @@
         <v>1867</v>
       </c>
       <c r="E695" s="5" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="F695" s="10">
-        <v>285</v>
+        <v>450</v>
       </c>
       <c r="G695" s="10">
         <v>1</v>
@@ -33358,19 +33340,25 @@
       <c r="I695">
         <v>3</v>
       </c>
-      <c r="Q695">
-        <v>1</v>
+      <c r="J695">
+        <v>4</v>
       </c>
       <c r="S695" t="s">
         <v>68</v>
       </c>
       <c r="T695" s="5" t="s">
-        <v>69</v>
+        <v>1888</v>
+      </c>
+      <c r="U695" t="s">
+        <v>68</v>
+      </c>
+      <c r="V695" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="696" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="B696" s="5" t="s">
         <v>331</v>
@@ -33382,10 +33370,10 @@
         <v>1867</v>
       </c>
       <c r="E696" s="5" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="F696" s="10">
-        <v>450</v>
+        <v>385</v>
       </c>
       <c r="G696" s="10">
         <v>1</v>
@@ -33393,11 +33381,8 @@
       <c r="H696">
         <v>2</v>
       </c>
-      <c r="I696">
-        <v>3</v>
-      </c>
-      <c r="J696">
-        <v>4</v>
+      <c r="Q696">
+        <v>1</v>
       </c>
       <c r="S696" t="s">
         <v>68</v>
@@ -33405,31 +33390,34 @@
       <c r="T696" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="U696" t="s">
-        <v>68</v>
-      </c>
-      <c r="V696" t="s">
+      <c r="AK696" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN696" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW696" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY696" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="697" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="B697" s="5" t="s">
-        <v>331</v>
+        <v>1924</v>
       </c>
       <c r="C697" s="5" t="s">
-        <v>331</v>
+        <v>1924</v>
       </c>
       <c r="D697" s="5" t="s">
-        <v>1867</v>
-      </c>
-      <c r="E697" s="5" t="s">
-        <v>1923</v>
+        <v>108</v>
       </c>
       <c r="F697" s="10">
-        <v>385</v>
+        <v>480</v>
       </c>
       <c r="G697" s="10">
         <v>1</v>
@@ -33437,55 +33425,37 @@
       <c r="H697">
         <v>2</v>
       </c>
-      <c r="Q697">
-        <v>1</v>
-      </c>
-      <c r="S697" t="s">
-        <v>68</v>
-      </c>
       <c r="T697" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="AK697" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN697" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW697" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY697" t="s">
+      <c r="U697" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="698" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="B698" s="5" t="s">
-        <v>1925</v>
+        <v>1383</v>
       </c>
       <c r="C698" s="5" t="s">
-        <v>1925</v>
+        <v>1382</v>
       </c>
       <c r="D698" s="5" t="s">
-        <v>108</v>
+        <v>1384</v>
       </c>
       <c r="F698" s="10">
-        <v>480</v>
+        <v>1</v>
       </c>
       <c r="G698" s="10">
         <v>1</v>
       </c>
-      <c r="H698">
-        <v>2</v>
+      <c r="S698" t="s">
+        <v>68</v>
       </c>
       <c r="T698" s="5" t="s">
         <v>1888</v>
-      </c>
-      <c r="U698" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="699" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33649,7 +33619,7 @@
         <v>1932</v>
       </c>
       <c r="B705" s="5" t="s">
-        <v>1383</v>
+        <v>1391</v>
       </c>
       <c r="C705" s="5" t="s">
         <v>1382</v>
@@ -33675,7 +33645,7 @@
         <v>1933</v>
       </c>
       <c r="B706" s="5" t="s">
-        <v>1391</v>
+        <v>1383</v>
       </c>
       <c r="C706" s="5" t="s">
         <v>1382</v>
@@ -33701,7 +33671,7 @@
         <v>1934</v>
       </c>
       <c r="B707" s="5" t="s">
-        <v>1383</v>
+        <v>1410</v>
       </c>
       <c r="C707" s="5" t="s">
         <v>1382</v>
@@ -33722,7 +33692,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="708" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
         <v>1935</v>
       </c>
@@ -33753,10 +33723,10 @@
         <v>1936</v>
       </c>
       <c r="B709" s="5" t="s">
-        <v>1410</v>
+        <v>1437</v>
       </c>
       <c r="C709" s="5" t="s">
-        <v>1382</v>
+        <v>1421</v>
       </c>
       <c r="D709" s="5" t="s">
         <v>1384</v>
@@ -33779,7 +33749,7 @@
         <v>1937</v>
       </c>
       <c r="B710" s="5" t="s">
-        <v>1437</v>
+        <v>1422</v>
       </c>
       <c r="C710" s="5" t="s">
         <v>1421</v>
@@ -33879,30 +33849,8 @@
       </c>
     </row>
     <row r="714" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A714" t="s">
-        <v>1941</v>
-      </c>
-      <c r="B714" s="5" t="s">
-        <v>1422</v>
-      </c>
-      <c r="C714" s="5" t="s">
-        <v>1421</v>
-      </c>
-      <c r="D714" s="5" t="s">
-        <v>1384</v>
-      </c>
-      <c r="F714" s="10">
-        <v>1</v>
-      </c>
-      <c r="G714" s="10">
-        <v>1</v>
-      </c>
-      <c r="S714" t="s">
-        <v>68</v>
-      </c>
-      <c r="T714" s="5" t="s">
-        <v>1888</v>
-      </c>
+      <c r="S714" s="4"/>
+      <c r="T714" s="4"/>
     </row>
     <row r="715" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S715" s="4"/>
@@ -35003,10 +34951,6 @@
     <row r="989" spans="19:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S989" s="4"/>
       <c r="T989" s="4"/>
-    </row>
-    <row r="990" spans="19:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S990" s="4"/>
-      <c r="T990" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>